<commit_message>
add email fetching, continue setup
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/REFrameworkNET5/StudioTemplates/REFramework/contentFiles/any/any/pt2/VisualBasic/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nsardonini\Documents\UiPath\Update Physical Asset History\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8C54E24-BA5C-4BF9-8DAB-2778512EC11B}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="56">
   <si>
     <t>Name</t>
   </si>
@@ -160,12 +159,45 @@
   </si>
   <si>
     <t>ProcessABCQueue</t>
+  </si>
+  <si>
+    <t>UITS</t>
+  </si>
+  <si>
+    <t>FinancePhysicalAssetHistory_Credentials</t>
+  </si>
+  <si>
+    <t>the name of the asset that holds the credentials for the Finance PSTST environment</t>
+  </si>
+  <si>
+    <t>FinancePhysicalAssetHistory_Environment</t>
+  </si>
+  <si>
+    <t>The Finance PSTST Environment</t>
+  </si>
+  <si>
+    <t>FinancePhysicalAssetHistory_LoginURL</t>
+  </si>
+  <si>
+    <t>The URL to log into Finance PSTST</t>
+  </si>
+  <si>
+    <t>FinancePhysicalAssetHistory_EmailToField</t>
+  </si>
+  <si>
+    <t>A list of semicolon-separated emails to send the start &amp; end emails to</t>
+  </si>
+  <si>
+    <t>FinancePhysicalAssetHistory_AutomationEnvironment</t>
+  </si>
+  <si>
+    <t>The environment of the automation, either UAT or Production</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -534,19 +566,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -594,7 +626,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
@@ -604,7 +636,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="28.8">
+    <row r="5" spans="1:26" ht="30">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1616,19 +1648,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1665,7 +1697,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1676,7 +1708,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1790,7 +1822,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="28.8">
+    <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -1801,7 +1833,17 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" t="s">
+        <v>47</v>
+      </c>
+    </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2779,17 +2821,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="2" width="50.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="65.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2828,10 +2872,62 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" t="s">
+        <v>55</v>
+      </c>
+    </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
work on add to queue process
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="2"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="65">
   <si>
     <t>Name</t>
   </si>
@@ -158,9 +158,6 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>ProcessABCQueue</t>
-  </si>
-  <si>
     <t>UITS</t>
   </si>
   <si>
@@ -192,6 +189,36 @@
   </si>
   <si>
     <t>The environment of the automation, either UAT or Production</t>
+  </si>
+  <si>
+    <t>FinancePhysicalAssetHistory_EmailSubject</t>
+  </si>
+  <si>
+    <t>FinancePhysicalAssetHistory_EmailIncomingFolderName</t>
+  </si>
+  <si>
+    <t>FinancePhysicalAssetHistory_LocalFolderName</t>
+  </si>
+  <si>
+    <t>FinancePhysicalAssetHistory_ProcessedFolderName</t>
+  </si>
+  <si>
+    <t>The subject of the email sent when submitting the form</t>
+  </si>
+  <si>
+    <t>The name of the folder that the email is sent to</t>
+  </si>
+  <si>
+    <t>The path of the folder that the excel file is saved to on the bot machine</t>
+  </si>
+  <si>
+    <t>The name of the folder that the email is moved to after processing</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>FinancePhysicalAssetHistory</t>
   </si>
 </sst>
 </file>
@@ -569,8 +596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -620,7 +647,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
@@ -654,7 +681,11 @@
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="B13" t="s">
+        <v>63</v>
+      </c>
+    </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1652,14 +1683,14 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="41" customWidth="1"/>
-    <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="1" max="1" width="63.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="100.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1708,7 +1739,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="30">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1822,7 +1853,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="45">
+    <row r="17" spans="1:3" ht="30">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -1835,13 +1866,13 @@
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" t="s">
         <v>46</v>
-      </c>
-      <c r="B18" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2824,13 +2855,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="50.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="59" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="65.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="26" width="65.42578125" customWidth="1"/>
@@ -2874,64 +2905,116 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
         <v>48</v>
-      </c>
-      <c r="B2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" t="s">
         <v>50</v>
-      </c>
-      <c r="B3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" t="s">
         <v>52</v>
-      </c>
-      <c r="B4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" t="s">
         <v>54</v>
       </c>
-      <c r="B5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" t="s">
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
         <v>55</v>
       </c>
+      <c r="B6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" t="s">
+        <v>62</v>
+      </c>
+    </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
set up transaction processing
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="65">
   <si>
     <t>Name</t>
   </si>
@@ -597,7 +597,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -657,7 +657,9 @@
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="C3" s="4" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
add workflows, config variable, screenshots
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="67">
   <si>
     <t>Name</t>
   </si>
@@ -219,6 +219,12 @@
   </si>
   <si>
     <t>FinancePhysicalAssetHistory</t>
+  </si>
+  <si>
+    <t>FinancePhysicalAssetHistory_LandingPageURL</t>
+  </si>
+  <si>
+    <t>Landing page for Finance PS</t>
   </si>
 </sst>
 </file>
@@ -596,7 +602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -2857,8 +2863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3017,7 +3023,20 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" t="s">
+        <v>66</v>
+      </c>
+    </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>